<commit_message>
Update database design schema (Excel only)   - Extend user table to include kills and deaths fields   - Extend sec_weapon, prime_weapon, and org tables with image URI field
Remove 'email=' assignment from createSession method. Email should be
populated automatically through relationship assignment.
</commit_message>
<xml_diff>
--- a/Modeling/Tables.xlsx
+++ b/Modeling/Tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>org</t>
   </si>
@@ -57,13 +57,73 @@
   </si>
   <si>
     <t>prime_weapon</t>
+  </si>
+  <si>
+    <t>mobility</t>
+  </si>
+  <si>
+    <t>image_url</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>op_id</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>administrator</t>
+  </si>
+  <si>
+    <t>IMPLEMENT CASCADING DELETES, UPDATES, ORPHAN DELETIONS, ETC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REFER TO SQLALCHEMY RELATIONSHIP DOCUMENTATION </t>
+  </si>
+  <si>
+    <t>string(email address)</t>
+  </si>
+  <si>
+    <t>string(URI)</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>= Primary Key</t>
+  </si>
+  <si>
+    <t>= Foreign Key</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>string(google user_id)</t>
+  </si>
+  <si>
+    <t>kills</t>
+  </si>
+  <si>
+    <t>deaths</t>
+  </si>
+  <si>
+    <t>ADD MATCH AND ROUND TABLES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,8 +146,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,8 +175,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -124,11 +205,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -143,10 +286,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -168,16 +366,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -209,7 +407,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1066800" y="419099"/>
+          <a:off x="2324100" y="295274"/>
           <a:ext cx="352425" cy="352425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -382,13 +580,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -435,13 +633,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -488,13 +686,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>790575</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -541,13 +739,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -594,13 +792,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>790575</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -634,6 +832,642 @@
       <xdr:spPr>
         <a:xfrm rot="5400000">
           <a:off x="1047750" y="2695574"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Graphic 10" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{719C9A37-7711-4FA5-BBC5-87972AA58814}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="6848475" y="1552575"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Graphic 11" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A661FCF-E2C8-4204-AABC-1C9910B810EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7019925" y="1552575"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Graphic 17" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{807C1A27-2AE5-451B-8FD2-C785A33B469E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7191375" y="1552575"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Graphic 18" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{072256B7-A5E9-49EC-96E8-F6DE4A9E9F90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1057275" y="3886199"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Graphic 19" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13051464-10EE-417D-935E-1AB94309F883}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5133975" y="285749"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Graphic 20" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65FCDB09-B252-44B8-A990-9C0BB00F28EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4714875" y="619124"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Graphic 21" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06F98EFD-DCDA-4B7A-AAF7-9EF3E8ABB0C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4924425" y="619124"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Graphic 22" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47A93C02-09F4-4957-A20C-967EE3DA6476}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5133975" y="619124"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Graphic 23" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B7CA467-689C-4C9B-A2EF-841465B315F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7134225" y="4210049"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Graphic 24" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AE8A9FD-D951-4BA3-9992-8B6F409EC41A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4448175" y="4219575"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Graphic 25" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A90BFA5-BA27-46B5-851F-3C49F4F1AF52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4619625" y="4219575"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Graphic 26" descr="Key">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A367CC93-A8E3-4F1B-943F-388DC0B53DF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4791075" y="4219575"/>
           <a:ext cx="352425" cy="352425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -943,10 +1777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816D9C45-7C77-4135-9BFA-2A8BA74FAD04}">
-  <dimension ref="B4:F19"/>
+  <dimension ref="B2:M29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,18 +1790,60 @@
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="7" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="4"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -977,85 +1853,401 @@
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E10" s="4" t="s">
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="5" t="s">
+      <c r="G12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="6"/>
+      <c r="D18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>